<commit_message>
added more things to pipeline
</commit_message>
<xml_diff>
--- a/files/Ateolpus-clust-tests.xlsx
+++ b/files/Ateolpus-clust-tests.xlsx
@@ -1,38 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patriciasalerno/Documents/Atelopus-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bioweb/Documents/P_Salerno/Atelopus-things/Atelopus/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D01739C-E71B-EC4B-8FD5-F2F8D4D9EABC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6A395A-C326-DA43-B349-E0B710AB5A6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="460" windowWidth="25800" windowHeight="15600" xr2:uid="{1AA8495C-B201-9B41-B0A7-985BD450CF38}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" activeTab="1" xr2:uid="{1AA8495C-B201-9B41-B0A7-985BD450CF38}"/>
   </bookViews>
   <sheets>
     <sheet name="clustering" sheetId="1" r:id="rId1"/>
     <sheet name="other-params" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'other-params'!$C$20:$C$24</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'other-params'!$D$19</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'other-params'!$D$20:$D$24</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>c86</t>
   </si>
@@ -125,6 +124,12 @@
   </si>
   <si>
     <t>22d</t>
+  </si>
+  <si>
+    <t>param20</t>
+  </si>
+  <si>
+    <t>loci</t>
   </si>
 </sst>
 </file>
@@ -1259,6 +1264,1162 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'other-params'!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>param20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'other-params'!$C$20:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A4F3-3849-8639-6064EB204EB6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'other-params'!$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>loci</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'other-params'!$D$20:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>85145</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109387</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>112892</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A4F3-3849-8639-6064EB204EB6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="863156304"/>
+        <c:axId val="863157984"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="863156304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="863157984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="863157984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="863156304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'other-params'!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>param20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'other-params'!$C$20:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A4F3-3849-8639-6064EB204EB6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'other-params'!$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>loci</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'other-params'!$D$20:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>85145</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109387</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>112892</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A4F3-3849-8639-6064EB204EB6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="863156304"/>
+        <c:axId val="863157984"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="863156304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="863157984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="863157984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="863156304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>max</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> SNPs per locus filter</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'other-params'!$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>loci</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'other-params'!$C$20:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'other-params'!$D$20:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>85145</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109387</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>112892</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A4F3-3849-8639-6064EB204EB6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="863156304"/>
+        <c:axId val="863157984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="863156304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="863157984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="863157984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="863156304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1339,6 +2500,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1843,6 +3124,1515 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2414,6 +5204,119 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE4BB046-B293-B14D-B2F5-E64BD7954D50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85ADE2F7-C569-0441-B1D0-A86B777B2043}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28BC8395-5415-5049-B57C-57B06C339BD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2721,8 +5624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC343AF7-CAD9-8544-AB6B-18E6EDDD93BD}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3096,10 +5999,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D56576-D852-A741-8516-56FE7FDF9EDD}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="144" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3241,7 +6144,56 @@
         <v>112892</v>
       </c>
     </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="1">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1">
+        <v>85145</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="1">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1">
+        <v>103859</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="1">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1">
+        <v>109387</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C23" s="1">
+        <v>18</v>
+      </c>
+      <c r="D23" s="1">
+        <v>112892</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C24" s="1">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>114954</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>